<commit_message>
Create new branch (v2)
Extends functionality to FODO and QMQ modules.
</commit_message>
<xml_diff>
--- a/Report_Log.xlsx
+++ b/Report_Log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\OneDrive\Desktop\Assembly Survey Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\APS-U\Assembly-Survey-Report-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE9BDAD-6AD7-440D-AA75-E5E833BE3876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0132A412-5BCE-4A2B-BB22-FD7A7EAA4115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1296,7 +1296,7 @@
   <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1421,201 +1421,201 @@
       <c r="A13" s="1"/>
       <c r="B13" s="5"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="5"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="5"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="5"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="5"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="5"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="5"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="B20" s="5"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+      <c r="B21" s="5"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="B22" s="5"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+      <c r="B23" s="5"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
+      <c r="B24" s="5"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
+      <c r="B25" s="5"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
+      <c r="B26" s="5"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
+      <c r="B29" s="5"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
+      <c r="B30" s="5"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
+      <c r="B31" s="5"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
+      <c r="B32" s="5"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
+      <c r="B33" s="5"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
+      <c r="B34" s="5"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
+      <c r="B35" s="5"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
+      <c r="B36" s="5"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
+      <c r="B37" s="5"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>

</xml_diff>

<commit_message>
Fixed typo in magnetModuleList
</commit_message>
<xml_diff>
--- a/Report_Log.xlsx
+++ b/Report_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Documents\Assembly-Survey-Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A05B147-6594-4D5C-B1F9-288E71AE1A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB838BD-608E-4598-9919-65819843D074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1296,7 +1296,7 @@
   <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>